<commit_message>
Updates to transmission capacity and GDP files
</commit_message>
<xml_diff>
--- a/InputData/io-model/BGDP/BAU GDP.xlsx
+++ b/InputData/io-model/BGDP/BAU GDP.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="23415" windowHeight="11310" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="38480" yWindow="7060" windowWidth="23420" windowHeight="11320" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="About" sheetId="1" state="visible" r:id="rId1"/>
@@ -11,7 +11,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BGDP" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -368,13 +368,13 @@
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col width="77.5703125" customWidth="1" style="7" min="2" max="2"/>
+    <col width="77.5" customWidth="1" style="7" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -488,18 +488,20 @@
   </sheetPr>
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col width="13.140625" customWidth="1" style="7" min="1" max="1"/>
+    <col width="13.1640625" customWidth="1" style="7" min="1" max="1"/>
     <col width="21" customWidth="1" style="7" min="2" max="2"/>
-    <col width="10.85546875" customWidth="1" style="7" min="3" max="3"/>
+    <col width="10.83203125" customWidth="1" style="7" min="3" max="3"/>
     <col width="13" customWidth="1" style="7" min="4" max="4"/>
-    <col width="13.28515625" customWidth="1" style="7" min="5" max="5"/>
-    <col width="17.140625" customWidth="1" style="7" min="7" max="7"/>
+    <col width="13.33203125" customWidth="1" style="7" min="5" max="5"/>
+    <col width="17.1640625" customWidth="1" style="7" min="7" max="7"/>
+    <col width="13.83203125" bestFit="1" customWidth="1" style="7" min="8" max="8"/>
+    <col width="11.83203125" bestFit="1" customWidth="1" style="7" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -535,7 +537,17 @@
       </c>
       <c r="G1" s="4" t="inlineStr">
         <is>
-          <t>Value</t>
+          <t>National GDP</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>National Growth</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>State GDP</t>
         </is>
       </c>
     </row>
@@ -571,6 +583,10 @@
       <c r="G2" t="n">
         <v>16208167.4518012</v>
       </c>
+      <c r="H2">
+        <f>G2/G2</f>
+        <v/>
+      </c>
       <c r="I2" t="n">
         <v>309239200000</v>
       </c>
@@ -607,6 +623,10 @@
       <c r="G3" s="5" t="n">
         <v>16671978.0010791</v>
       </c>
+      <c r="H3">
+        <f>G3/G2</f>
+        <v/>
+      </c>
       <c r="I3" t="n">
         <v>313086200000</v>
       </c>
@@ -643,6 +663,10 @@
       <c r="G4" t="n">
         <v>16919603.4177135</v>
       </c>
+      <c r="H4">
+        <f>G4/G3</f>
+        <v/>
+      </c>
       <c r="I4" t="n">
         <v>319129900000</v>
       </c>
@@ -679,6 +703,10 @@
       <c r="G5" t="n">
         <v>17304243.0256237</v>
       </c>
+      <c r="H5">
+        <f>G5/G4</f>
+        <v/>
+      </c>
       <c r="I5" t="n">
         <v>325322700000</v>
       </c>
@@ -715,6 +743,10 @@
       <c r="G6" t="n">
         <v>17798638.6604435</v>
       </c>
+      <c r="H6">
+        <f>G6/G5</f>
+        <v/>
+      </c>
       <c r="I6" t="n">
         <v>333919500000</v>
       </c>
@@ -751,6 +783,10 @@
       <c r="G7" t="n">
         <v>18292645.5693758</v>
       </c>
+      <c r="H7">
+        <f>G7/G6</f>
+        <v/>
+      </c>
       <c r="I7" t="n">
         <v>338752300000</v>
       </c>
@@ -787,6 +823,14 @@
       <c r="G8" t="n">
         <v>18587190</v>
       </c>
+      <c r="H8">
+        <f>G8/G7</f>
+        <v/>
+      </c>
+      <c r="I8">
+        <f>I7*H8</f>
+        <v/>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -820,6 +864,14 @@
       <c r="G9" t="n">
         <v>18849540</v>
       </c>
+      <c r="H9">
+        <f>G9/G8</f>
+        <v/>
+      </c>
+      <c r="I9">
+        <f>I8*H9</f>
+        <v/>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -853,6 +905,14 @@
       <c r="G10" t="n">
         <v>19124900</v>
       </c>
+      <c r="H10">
+        <f>G10/G9</f>
+        <v/>
+      </c>
+      <c r="I10">
+        <f>I9*H10</f>
+        <v/>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -886,6 +946,14 @@
       <c r="G11" t="n">
         <v>19422190</v>
       </c>
+      <c r="H11">
+        <f>G11/G10</f>
+        <v/>
+      </c>
+      <c r="I11">
+        <f>I10*H11</f>
+        <v/>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -919,6 +987,14 @@
       <c r="G12" t="n">
         <v>19740540</v>
       </c>
+      <c r="H12">
+        <f>G12/G11</f>
+        <v/>
+      </c>
+      <c r="I12">
+        <f>I11*H12</f>
+        <v/>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -952,6 +1028,14 @@
       <c r="G13" t="n">
         <v>20075600</v>
       </c>
+      <c r="H13">
+        <f>G13/G12</f>
+        <v/>
+      </c>
+      <c r="I13">
+        <f>I12*H13</f>
+        <v/>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -985,6 +1069,14 @@
       <c r="G14" t="n">
         <v>20424180</v>
       </c>
+      <c r="H14">
+        <f>G14/G13</f>
+        <v/>
+      </c>
+      <c r="I14">
+        <f>I13*H14</f>
+        <v/>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1018,6 +1110,14 @@
       <c r="G15" t="n">
         <v>20784020</v>
       </c>
+      <c r="H15">
+        <f>G15/G14</f>
+        <v/>
+      </c>
+      <c r="I15">
+        <f>I14*H15</f>
+        <v/>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1051,6 +1151,14 @@
       <c r="G16" t="n">
         <v>21153450</v>
       </c>
+      <c r="H16">
+        <f>G16/G15</f>
+        <v/>
+      </c>
+      <c r="I16">
+        <f>I15*H16</f>
+        <v/>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1084,6 +1192,14 @@
       <c r="G17" t="n">
         <v>21531180</v>
       </c>
+      <c r="H17">
+        <f>G17/G16</f>
+        <v/>
+      </c>
+      <c r="I17">
+        <f>I16*H17</f>
+        <v/>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1117,6 +1233,14 @@
       <c r="G18" t="n">
         <v>21916430</v>
       </c>
+      <c r="H18">
+        <f>G18/G17</f>
+        <v/>
+      </c>
+      <c r="I18">
+        <f>I17*H18</f>
+        <v/>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1150,6 +1274,14 @@
       <c r="G19" t="n">
         <v>22309050</v>
       </c>
+      <c r="H19">
+        <f>G19/G18</f>
+        <v/>
+      </c>
+      <c r="I19">
+        <f>I18*H19</f>
+        <v/>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1183,6 +1315,14 @@
       <c r="G20" t="n">
         <v>22709530</v>
       </c>
+      <c r="H20">
+        <f>G20/G19</f>
+        <v/>
+      </c>
+      <c r="I20">
+        <f>I19*H20</f>
+        <v/>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1216,6 +1356,14 @@
       <c r="G21" t="n">
         <v>23118740</v>
       </c>
+      <c r="H21">
+        <f>G21/G20</f>
+        <v/>
+      </c>
+      <c r="I21">
+        <f>I20*H21</f>
+        <v/>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1249,6 +1397,14 @@
       <c r="G22" t="n">
         <v>23537610</v>
       </c>
+      <c r="H22">
+        <f>G22/G21</f>
+        <v/>
+      </c>
+      <c r="I22">
+        <f>I21*H22</f>
+        <v/>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1282,6 +1438,14 @@
       <c r="G23" t="n">
         <v>23967030</v>
       </c>
+      <c r="H23">
+        <f>G23/G22</f>
+        <v/>
+      </c>
+      <c r="I23">
+        <f>I22*H23</f>
+        <v/>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1315,6 +1479,14 @@
       <c r="G24" t="n">
         <v>24407860</v>
       </c>
+      <c r="H24">
+        <f>G24/G23</f>
+        <v/>
+      </c>
+      <c r="I24">
+        <f>I23*H24</f>
+        <v/>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1348,6 +1520,14 @@
       <c r="G25" t="n">
         <v>24861010</v>
       </c>
+      <c r="H25">
+        <f>G25/G24</f>
+        <v/>
+      </c>
+      <c r="I25">
+        <f>I24*H25</f>
+        <v/>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1381,6 +1561,14 @@
       <c r="G26" t="n">
         <v>25327180</v>
       </c>
+      <c r="H26">
+        <f>G26/G25</f>
+        <v/>
+      </c>
+      <c r="I26">
+        <f>I25*H26</f>
+        <v/>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1414,6 +1602,14 @@
       <c r="G27" t="n">
         <v>25806800</v>
       </c>
+      <c r="H27">
+        <f>G27/G26</f>
+        <v/>
+      </c>
+      <c r="I27">
+        <f>I26*H27</f>
+        <v/>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1447,6 +1643,14 @@
       <c r="G28" t="n">
         <v>26300140</v>
       </c>
+      <c r="H28">
+        <f>G28/G27</f>
+        <v/>
+      </c>
+      <c r="I28">
+        <f>I27*H28</f>
+        <v/>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1480,6 +1684,14 @@
       <c r="G29" t="n">
         <v>26807420</v>
       </c>
+      <c r="H29">
+        <f>G29/G28</f>
+        <v/>
+      </c>
+      <c r="I29">
+        <f>I28*H29</f>
+        <v/>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1513,6 +1725,14 @@
       <c r="G30" t="n">
         <v>27328940</v>
       </c>
+      <c r="H30">
+        <f>G30/G29</f>
+        <v/>
+      </c>
+      <c r="I30">
+        <f>I29*H30</f>
+        <v/>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1546,6 +1766,14 @@
       <c r="G31" t="n">
         <v>27864750</v>
       </c>
+      <c r="H31">
+        <f>G31/G30</f>
+        <v/>
+      </c>
+      <c r="I31">
+        <f>I30*H31</f>
+        <v/>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1579,6 +1807,14 @@
       <c r="G32" t="n">
         <v>28414590</v>
       </c>
+      <c r="H32">
+        <f>G32/G31</f>
+        <v/>
+      </c>
+      <c r="I32">
+        <f>I31*H32</f>
+        <v/>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1612,6 +1848,14 @@
       <c r="G33" t="n">
         <v>28978050</v>
       </c>
+      <c r="H33">
+        <f>G33/G32</f>
+        <v/>
+      </c>
+      <c r="I33">
+        <f>I32*H33</f>
+        <v/>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1645,6 +1889,14 @@
       <c r="G34" t="n">
         <v>29554850</v>
       </c>
+      <c r="H34">
+        <f>G34/G33</f>
+        <v/>
+      </c>
+      <c r="I34">
+        <f>I33*H34</f>
+        <v/>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1678,6 +1930,14 @@
       <c r="G35" t="n">
         <v>30144870</v>
       </c>
+      <c r="H35">
+        <f>G35/G34</f>
+        <v/>
+      </c>
+      <c r="I35">
+        <f>I34*H35</f>
+        <v/>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1711,6 +1971,14 @@
       <c r="G36" t="n">
         <v>30747840</v>
       </c>
+      <c r="H36">
+        <f>G36/G35</f>
+        <v/>
+      </c>
+      <c r="I36">
+        <f>I35*H36</f>
+        <v/>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1744,6 +2012,14 @@
       <c r="G37" t="n">
         <v>31363330</v>
       </c>
+      <c r="H37">
+        <f>G37/G36</f>
+        <v/>
+      </c>
+      <c r="I37">
+        <f>I36*H37</f>
+        <v/>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1777,6 +2053,14 @@
       <c r="G38" t="n">
         <v>31990910</v>
       </c>
+      <c r="H38">
+        <f>G38/G37</f>
+        <v/>
+      </c>
+      <c r="I38">
+        <f>I37*H38</f>
+        <v/>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1810,6 +2094,14 @@
       <c r="G39" t="n">
         <v>32630430</v>
       </c>
+      <c r="H39">
+        <f>G39/G38</f>
+        <v/>
+      </c>
+      <c r="I39">
+        <f>I38*H39</f>
+        <v/>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1843,6 +2135,14 @@
       <c r="G40" t="n">
         <v>33282110</v>
       </c>
+      <c r="H40">
+        <f>G40/G39</f>
+        <v/>
+      </c>
+      <c r="I40">
+        <f>I39*H40</f>
+        <v/>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1876,6 +2176,14 @@
       <c r="G41" t="n">
         <v>33946130</v>
       </c>
+      <c r="H41">
+        <f>G41/G40</f>
+        <v/>
+      </c>
+      <c r="I41">
+        <f>I40*H41</f>
+        <v/>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1909,6 +2217,14 @@
       <c r="G42" t="n">
         <v>34622620</v>
       </c>
+      <c r="H42">
+        <f>G42/G41</f>
+        <v/>
+      </c>
+      <c r="I42">
+        <f>I41*H42</f>
+        <v/>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1942,6 +2258,14 @@
       <c r="G43" t="n">
         <v>35311770</v>
       </c>
+      <c r="H43">
+        <f>G43/G42</f>
+        <v/>
+      </c>
+      <c r="I43">
+        <f>I42*H43</f>
+        <v/>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1975,6 +2299,14 @@
       <c r="G44" t="n">
         <v>36014100</v>
       </c>
+      <c r="H44">
+        <f>G44/G43</f>
+        <v/>
+      </c>
+      <c r="I44">
+        <f>I43*H44</f>
+        <v/>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2008,6 +2340,14 @@
       <c r="G45" t="n">
         <v>36730540</v>
       </c>
+      <c r="H45">
+        <f>G45/G44</f>
+        <v/>
+      </c>
+      <c r="I45">
+        <f>I44*H45</f>
+        <v/>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2041,6 +2381,14 @@
       <c r="G46" t="n">
         <v>37462060</v>
       </c>
+      <c r="H46">
+        <f>G46/G45</f>
+        <v/>
+      </c>
+      <c r="I46">
+        <f>I45*H46</f>
+        <v/>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2074,6 +2422,14 @@
       <c r="G47" t="n">
         <v>38209630</v>
       </c>
+      <c r="H47">
+        <f>G47/G46</f>
+        <v/>
+      </c>
+      <c r="I47">
+        <f>I46*H47</f>
+        <v/>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2106,6 +2462,14 @@
       </c>
       <c r="G48" t="n">
         <v>38974320</v>
+      </c>
+      <c r="H48">
+        <f>G48/G47</f>
+        <v/>
+      </c>
+      <c r="I48">
+        <f>I47*H48</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -2122,14 +2486,14 @@
   </sheetPr>
   <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col width="17.7109375" customWidth="1" style="7" min="1" max="1"/>
-    <col width="15.140625" customWidth="1" style="7" min="2" max="2"/>
+    <col width="17.6640625" customWidth="1" style="7" min="1" max="1"/>
+    <col width="15.1640625" customWidth="1" style="7" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2149,7 +2513,7 @@
         <v>2014</v>
       </c>
       <c r="B2">
-        <f>'OECD Data'!G2*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I2</f>
         <v/>
       </c>
     </row>
@@ -2158,7 +2522,7 @@
         <v>2015</v>
       </c>
       <c r="B3">
-        <f>'OECD Data'!G3*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I3</f>
         <v/>
       </c>
     </row>
@@ -2167,7 +2531,7 @@
         <v>2016</v>
       </c>
       <c r="B4">
-        <f>'OECD Data'!G4*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I4</f>
         <v/>
       </c>
     </row>
@@ -2176,7 +2540,7 @@
         <v>2017</v>
       </c>
       <c r="B5">
-        <f>'OECD Data'!G5*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I5</f>
         <v/>
       </c>
     </row>
@@ -2185,7 +2549,7 @@
         <v>2018</v>
       </c>
       <c r="B6">
-        <f>'OECD Data'!G6*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I6</f>
         <v/>
       </c>
     </row>
@@ -2194,7 +2558,7 @@
         <v>2019</v>
       </c>
       <c r="B7">
-        <f>'OECD Data'!G7*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I7</f>
         <v/>
       </c>
     </row>
@@ -2203,7 +2567,7 @@
         <v>2020</v>
       </c>
       <c r="B8">
-        <f>'OECD Data'!G8*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I8</f>
         <v/>
       </c>
     </row>
@@ -2212,7 +2576,7 @@
         <v>2021</v>
       </c>
       <c r="B9">
-        <f>'OECD Data'!G9*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I9</f>
         <v/>
       </c>
     </row>
@@ -2221,7 +2585,7 @@
         <v>2022</v>
       </c>
       <c r="B10">
-        <f>'OECD Data'!G10*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I10</f>
         <v/>
       </c>
     </row>
@@ -2230,7 +2594,7 @@
         <v>2023</v>
       </c>
       <c r="B11">
-        <f>'OECD Data'!G11*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I11</f>
         <v/>
       </c>
     </row>
@@ -2239,7 +2603,7 @@
         <v>2024</v>
       </c>
       <c r="B12">
-        <f>'OECD Data'!G12*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I12</f>
         <v/>
       </c>
     </row>
@@ -2248,7 +2612,7 @@
         <v>2025</v>
       </c>
       <c r="B13">
-        <f>'OECD Data'!G13*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I13</f>
         <v/>
       </c>
     </row>
@@ -2257,7 +2621,7 @@
         <v>2026</v>
       </c>
       <c r="B14">
-        <f>'OECD Data'!G14*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I14</f>
         <v/>
       </c>
     </row>
@@ -2266,7 +2630,7 @@
         <v>2027</v>
       </c>
       <c r="B15">
-        <f>'OECD Data'!G15*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I15</f>
         <v/>
       </c>
     </row>
@@ -2275,7 +2639,7 @@
         <v>2028</v>
       </c>
       <c r="B16">
-        <f>'OECD Data'!G16*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I16</f>
         <v/>
       </c>
     </row>
@@ -2284,7 +2648,7 @@
         <v>2029</v>
       </c>
       <c r="B17">
-        <f>'OECD Data'!G17*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I17</f>
         <v/>
       </c>
     </row>
@@ -2293,7 +2657,7 @@
         <v>2030</v>
       </c>
       <c r="B18">
-        <f>'OECD Data'!G18*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I18</f>
         <v/>
       </c>
     </row>
@@ -2302,7 +2666,7 @@
         <v>2031</v>
       </c>
       <c r="B19">
-        <f>'OECD Data'!G19*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I19</f>
         <v/>
       </c>
     </row>
@@ -2311,7 +2675,7 @@
         <v>2032</v>
       </c>
       <c r="B20">
-        <f>'OECD Data'!G20*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I20</f>
         <v/>
       </c>
     </row>
@@ -2320,7 +2684,7 @@
         <v>2033</v>
       </c>
       <c r="B21">
-        <f>'OECD Data'!G21*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I21</f>
         <v/>
       </c>
     </row>
@@ -2329,7 +2693,7 @@
         <v>2034</v>
       </c>
       <c r="B22">
-        <f>'OECD Data'!G22*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I22</f>
         <v/>
       </c>
     </row>
@@ -2338,7 +2702,7 @@
         <v>2035</v>
       </c>
       <c r="B23">
-        <f>'OECD Data'!G23*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I23</f>
         <v/>
       </c>
     </row>
@@ -2347,7 +2711,7 @@
         <v>2036</v>
       </c>
       <c r="B24">
-        <f>'OECD Data'!G24*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I24</f>
         <v/>
       </c>
     </row>
@@ -2356,7 +2720,7 @@
         <v>2037</v>
       </c>
       <c r="B25">
-        <f>'OECD Data'!G25*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I25</f>
         <v/>
       </c>
     </row>
@@ -2365,7 +2729,7 @@
         <v>2038</v>
       </c>
       <c r="B26">
-        <f>'OECD Data'!G26*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I26</f>
         <v/>
       </c>
     </row>
@@ -2374,7 +2738,7 @@
         <v>2039</v>
       </c>
       <c r="B27">
-        <f>'OECD Data'!G27*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I27</f>
         <v/>
       </c>
     </row>
@@ -2383,7 +2747,7 @@
         <v>2040</v>
       </c>
       <c r="B28">
-        <f>'OECD Data'!G28*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I28</f>
         <v/>
       </c>
     </row>
@@ -2392,7 +2756,7 @@
         <v>2041</v>
       </c>
       <c r="B29">
-        <f>'OECD Data'!G29*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I29</f>
         <v/>
       </c>
     </row>
@@ -2401,7 +2765,7 @@
         <v>2042</v>
       </c>
       <c r="B30">
-        <f>'OECD Data'!G30*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I30</f>
         <v/>
       </c>
     </row>
@@ -2410,7 +2774,7 @@
         <v>2043</v>
       </c>
       <c r="B31">
-        <f>'OECD Data'!G31*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I31</f>
         <v/>
       </c>
     </row>
@@ -2419,7 +2783,7 @@
         <v>2044</v>
       </c>
       <c r="B32">
-        <f>'OECD Data'!G32*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I32</f>
         <v/>
       </c>
     </row>
@@ -2428,7 +2792,7 @@
         <v>2045</v>
       </c>
       <c r="B33">
-        <f>'OECD Data'!G33*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I33</f>
         <v/>
       </c>
     </row>
@@ -2437,7 +2801,7 @@
         <v>2046</v>
       </c>
       <c r="B34">
-        <f>'OECD Data'!G34*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I34</f>
         <v/>
       </c>
     </row>
@@ -2446,7 +2810,7 @@
         <v>2047</v>
       </c>
       <c r="B35">
-        <f>'OECD Data'!G35*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I35</f>
         <v/>
       </c>
     </row>
@@ -2455,7 +2819,7 @@
         <v>2048</v>
       </c>
       <c r="B36">
-        <f>'OECD Data'!G36*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I36</f>
         <v/>
       </c>
     </row>
@@ -2464,7 +2828,7 @@
         <v>2049</v>
       </c>
       <c r="B37">
-        <f>'OECD Data'!G37*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I37</f>
         <v/>
       </c>
     </row>
@@ -2473,7 +2837,7 @@
         <v>2050</v>
       </c>
       <c r="B38">
-        <f>'OECD Data'!G38*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I38</f>
         <v/>
       </c>
     </row>
@@ -2482,7 +2846,7 @@
         <v>2051</v>
       </c>
       <c r="B39">
-        <f>'OECD Data'!G39*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I39</f>
         <v/>
       </c>
     </row>
@@ -2491,7 +2855,7 @@
         <v>2052</v>
       </c>
       <c r="B40">
-        <f>'OECD Data'!G40*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I40</f>
         <v/>
       </c>
     </row>
@@ -2500,7 +2864,7 @@
         <v>2053</v>
       </c>
       <c r="B41">
-        <f>'OECD Data'!G41*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I41</f>
         <v/>
       </c>
     </row>
@@ -2509,7 +2873,7 @@
         <v>2054</v>
       </c>
       <c r="B42">
-        <f>'OECD Data'!G42*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I42</f>
         <v/>
       </c>
     </row>
@@ -2518,7 +2882,7 @@
         <v>2055</v>
       </c>
       <c r="B43">
-        <f>'OECD Data'!G43*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I43</f>
         <v/>
       </c>
     </row>
@@ -2527,7 +2891,7 @@
         <v>2056</v>
       </c>
       <c r="B44">
-        <f>'OECD Data'!G44*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I44</f>
         <v/>
       </c>
     </row>
@@ -2536,7 +2900,7 @@
         <v>2057</v>
       </c>
       <c r="B45">
-        <f>'OECD Data'!G45*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I45</f>
         <v/>
       </c>
     </row>
@@ -2545,7 +2909,7 @@
         <v>2058</v>
       </c>
       <c r="B46">
-        <f>'OECD Data'!G46*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I46</f>
         <v/>
       </c>
     </row>
@@ -2554,7 +2918,7 @@
         <v>2059</v>
       </c>
       <c r="B47">
-        <f>'OECD Data'!G47*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I47</f>
         <v/>
       </c>
     </row>
@@ -2563,7 +2927,7 @@
         <v>2060</v>
       </c>
       <c r="B48">
-        <f>'OECD Data'!G48*About!$A$15*About!$A$16</f>
+        <f>'OECD Data'!I48</f>
         <v/>
       </c>
     </row>

</xml_diff>